<commit_message>
Synchronized with the demo rep
</commit_message>
<xml_diff>
--- a/TC_CreateCustomerGroup/Main.rvl.xlsx
+++ b/TC_CreateCustomerGroup/Main.rvl.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="156">
   <si>
     <t>Flow</t>
   </si>
@@ -447,6 +447,42 @@
   </si>
   <si>
     <t>IT2</t>
+  </si>
+  <si>
+    <t>GetRowCount</t>
+  </si>
+  <si>
+    <t>GetCell</t>
+  </si>
+  <si>
+    <t>CustGroup</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>param1 != param2</t>
+  </si>
+  <si>
+    <t>DFO</t>
+  </si>
+  <si>
+    <t>Launch</t>
+  </si>
+  <si>
+    <t>PassWelcomeScreen</t>
+  </si>
+  <si>
+    <t>SearchPage</t>
+  </si>
+  <si>
+    <t>DoTrim</t>
+  </si>
+  <si>
+    <t>str</t>
+  </si>
+  <si>
+    <t>120000</t>
   </si>
 </sst>
 </file>
@@ -467,7 +503,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="582">
+  <borders count="611">
     <border>
       <left/>
       <right/>
@@ -1056,11 +1092,40 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="582">
+  <cellXfs count="611">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -1643,6 +1708,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="579" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="580" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="581" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="582" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="583" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="584" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="585" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="586" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="587" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="588" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="589" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="590" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="591" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="592" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="593" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="594" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="595" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="596" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="597" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="598" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="599" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="600" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="601" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="602" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="603" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="604" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="605" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="606" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="607" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="608" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="609" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="610" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1652,7 +1746,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H41"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.453125" customWidth="true"/>
@@ -1806,399 +1900,583 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="460"/>
+      <c r="A9" s="457" t="s">
+        <v>67</v>
+      </c>
       <c r="B9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="447"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="17"/>
+      <c r="B11" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="24"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="25"/>
+      <c r="B12" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="32"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="33"/>
+      <c r="B13" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" s="36" t="s">
+        <v>152</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="H13" s="40"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="435"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="607"/>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" t="s">
+        <v>94</v>
+      </c>
+      <c r="G15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="608"/>
+      <c r="B16" t="s">
         <v>24</v>
       </c>
-      <c r="E9" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="E16" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" t="s">
         <v>38</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="609"/>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="582"/>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>141</v>
+      </c>
+      <c r="D18" t="s">
+        <v>145</v>
+      </c>
+      <c r="E18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="461"/>
-      <c r="B10" t="s">
+    <row r="19">
+      <c r="A19" s="599"/>
+      <c r="B19" t="s">
         <v>24</v>
       </c>
-      <c r="E10" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="E19" t="s">
+        <v>121</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="600"/>
+      <c r="B20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F20" t="s">
+        <v>105</v>
+      </c>
+      <c r="G20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="604" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" t="s">
+        <v>153</v>
+      </c>
+      <c r="E21" t="s">
+        <v>154</v>
+      </c>
+      <c r="F21" t="s">
+        <v>105</v>
+      </c>
+      <c r="G21" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="605" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>113</v>
+      </c>
+      <c r="F22" t="s">
+        <v>105</v>
+      </c>
+      <c r="G22" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="606"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="595"/>
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" t="s">
+        <v>104</v>
+      </c>
+      <c r="F24" t="s">
+        <v>105</v>
+      </c>
+      <c r="G24" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="583" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" t="s">
+        <v>85</v>
+      </c>
+      <c r="F25" t="s">
+        <v>105</v>
+      </c>
+      <c r="G25" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="585" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>148</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="586" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
+        <v>89</v>
+      </c>
+      <c r="F27" t="s">
+        <v>70</v>
+      </c>
+      <c r="G27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="587" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="504" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>135</v>
+      </c>
+      <c r="D29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="574" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>141</v>
+      </c>
+      <c r="D30" t="s">
+        <v>119</v>
+      </c>
+      <c r="E30" t="s">
+        <v>120</v>
+      </c>
+      <c r="F30" t="s">
         <v>38</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G30" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="462"/>
-      <c r="B11" t="s">
+    <row r="31">
+      <c r="A31" s="575" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" t="s">
         <v>24</v>
       </c>
-      <c r="E11" t="s">
-        <v>79</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" t="s">
+        <v>121</v>
+      </c>
+      <c r="F31" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="576" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>141</v>
+      </c>
+      <c r="D32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="577" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>141</v>
+      </c>
+      <c r="D33" t="s">
+        <v>119</v>
+      </c>
+      <c r="E33" t="s">
+        <v>120</v>
+      </c>
+      <c r="F33" t="s">
         <v>38</v>
       </c>
-      <c r="G11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="463"/>
-      <c r="B12" t="s">
+      <c r="G33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="578" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
         <v>24</v>
       </c>
-      <c r="E12" t="s">
-        <v>81</v>
-      </c>
-      <c r="F12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="457" t="s">
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" t="s">
+        <v>121</v>
+      </c>
+      <c r="F34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="579" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>139</v>
+      </c>
+      <c r="D35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="593" t="s">
         <v>67</v>
       </c>
-      <c r="B13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="447"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="17"/>
-      <c r="B15" s="18" t="s">
+      <c r="B36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="592"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="580" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="H15" s="24"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="25"/>
-      <c r="B16" s="26" t="s">
+      <c r="C38" t="s">
+        <v>140</v>
+      </c>
+      <c r="D38" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="581"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="499"/>
+      <c r="B40" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="H16" s="32"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="33"/>
-      <c r="B17" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="38" t="s">
+      <c r="C40" t="s">
+        <v>127</v>
+      </c>
+      <c r="D40" t="s">
+        <v>128</v>
+      </c>
+      <c r="E40" t="s">
+        <v>74</v>
+      </c>
+      <c r="F40" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="39" t="s">
-        <v>133</v>
-      </c>
-      <c r="H17" s="40"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="435"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="504" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" t="s">
-        <v>135</v>
-      </c>
-      <c r="D19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="574" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" t="s">
-        <v>141</v>
-      </c>
-      <c r="D20" t="s">
-        <v>119</v>
-      </c>
-      <c r="E20" t="s">
-        <v>120</v>
-      </c>
-      <c r="F20" t="s">
-        <v>38</v>
-      </c>
-      <c r="G20" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="575" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" t="s">
-        <v>121</v>
-      </c>
-      <c r="F21" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="576" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" t="s">
-        <v>141</v>
-      </c>
-      <c r="D22" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22" t="s">
-        <v>70</v>
-      </c>
-      <c r="G22" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="577" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" t="s">
-        <v>141</v>
-      </c>
-      <c r="D23" t="s">
-        <v>119</v>
-      </c>
-      <c r="E23" t="s">
-        <v>120</v>
-      </c>
-      <c r="F23" t="s">
-        <v>38</v>
-      </c>
-      <c r="G23" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="578" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" t="s">
-        <v>121</v>
-      </c>
-      <c r="F24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="579" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" t="s">
-        <v>139</v>
-      </c>
-      <c r="D25" t="s">
-        <v>44</v>
-      </c>
-      <c r="E25" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" t="s">
-        <v>7</v>
-      </c>
-      <c r="G25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="580" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" t="s">
-        <v>140</v>
-      </c>
-      <c r="D26" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="581"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="499"/>
-      <c r="B28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" t="s">
-        <v>127</v>
-      </c>
-      <c r="D28" t="s">
-        <v>128</v>
-      </c>
-      <c r="E28" t="s">
-        <v>74</v>
-      </c>
-      <c r="F28" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" t="s">
+      <c r="G40" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="145"/>
-      <c r="B29" s="146" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" s="147" t="s">
-        <v>98</v>
-      </c>
-      <c r="D29" s="148" t="s">
-        <v>99</v>
-      </c>
-      <c r="E29" s="149" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="150" t="s">
-        <v>7</v>
-      </c>
-      <c r="G29" s="151" t="s">
-        <v>7</v>
-      </c>
-      <c r="H29" s="152"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="153"/>
-      <c r="B30" s="154"/>
-      <c r="C30" s="155"/>
-      <c r="D30" s="156"/>
-      <c r="E30" s="157"/>
-      <c r="F30" s="158"/>
-      <c r="G30" s="159"/>
-      <c r="H30" s="160"/>
+    <row r="41">
+      <c r="A41" s="153"/>
+      <c r="B41" s="154"/>
+      <c r="C41" s="155"/>
+      <c r="D41" s="156"/>
+      <c r="E41" s="157"/>
+      <c r="F41" s="158"/>
+      <c r="G41" s="159"/>
+      <c r="H41" s="160"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>